<commit_message>
added (thousands) to DM_POP_TOT_AGE name description
</commit_message>
<xml_diff>
--- a/tmee/data_in/data_dictionary/indicator_dictionary_TM_v5.xlsx
+++ b/tmee/data_in/data_dictionary/indicator_dictionary_TM_v5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/16f1c7c3db740efb/UNICEF/TransMonEE/data-etl/tmee/data_in/data_dictionary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="154" documentId="13_ncr:1_{0D7C4ACD-3B96-48F3-99D4-5E393553EB86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{89FDB992-444E-4F26-BB5F-C47141965BEF}"/>
+  <xr:revisionPtr revIDLastSave="157" documentId="13_ncr:1_{0D7C4ACD-3B96-48F3-99D4-5E393553EB86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8806B824-3422-47AE-B502-27CA73A00B97}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Snapshot" sheetId="1" r:id="rId1"/>
@@ -8728,9 +8728,6 @@
     <t>UNPD population</t>
   </si>
   <si>
-    <t>Total population by age</t>
-  </si>
-  <si>
     <t>DM_POP_TOT_AGE</t>
   </si>
   <si>
@@ -8816,6 +8813,9 @@
   </si>
   <si>
     <t>S-232</t>
+  </si>
+  <si>
+    <t>Total population by age (expressed in thousands)</t>
   </si>
 </sst>
 </file>
@@ -9562,7 +9562,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L224"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A211" workbookViewId="0">
+    <sheetView topLeftCell="A211" workbookViewId="0">
       <selection activeCell="H222" sqref="H222:H224"/>
     </sheetView>
   </sheetViews>
@@ -9699,7 +9699,7 @@
       </c>
       <c r="C4" s="33" t="str">
         <f>VLOOKUP(B4,Indicator!$A$2:$F$105,5,FALSE)</f>
-        <v>Total population by age</v>
+        <v>Total population by age (expressed in thousands)</v>
       </c>
       <c r="D4" s="25" t="str">
         <f>VLOOKUP(B4,Indicator!$A$2:$F$105,6,FALSE)</f>
@@ -17039,7 +17039,7 @@
     </row>
     <row r="221" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A221" s="1" t="s">
-        <v>2900</v>
+        <v>2899</v>
       </c>
       <c r="B221" s="16" t="s">
         <v>1440</v>
@@ -17072,7 +17072,7 @@
     </row>
     <row r="222" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A222" s="1" t="s">
-        <v>2915</v>
+        <v>2914</v>
       </c>
       <c r="B222" s="16" t="s">
         <v>1443</v>
@@ -17105,7 +17105,7 @@
     </row>
     <row r="223" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A223" s="1" t="s">
-        <v>2916</v>
+        <v>2915</v>
       </c>
       <c r="B223" s="16" t="s">
         <v>1818</v>
@@ -17138,7 +17138,7 @@
     </row>
     <row r="224" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A224" s="1" t="s">
-        <v>2917</v>
+        <v>2916</v>
       </c>
       <c r="B224" s="16" t="s">
         <v>1820</v>
@@ -17706,9 +17706,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M645"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A273" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A276" sqref="A276:A645"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -18284,10 +18284,10 @@
         <v>2893</v>
       </c>
       <c r="E23" s="33" t="s">
+        <v>2923</v>
+      </c>
+      <c r="F23" s="56" t="s">
         <v>2894</v>
-      </c>
-      <c r="F23" s="56" t="s">
-        <v>2895</v>
       </c>
       <c r="M23" s="36"/>
     </row>
@@ -23380,10 +23380,10 @@
         <v>2843</v>
       </c>
       <c r="E272" s="50" t="s">
-        <v>2904</v>
+        <v>2903</v>
       </c>
       <c r="F272" t="s">
-        <v>2903</v>
+        <v>2902</v>
       </c>
     </row>
     <row r="273" spans="1:10" x14ac:dyDescent="0.35">
@@ -23400,10 +23400,10 @@
         <v>2423</v>
       </c>
       <c r="E273" s="50" t="s">
-        <v>2908</v>
+        <v>2907</v>
       </c>
       <c r="F273" t="s">
-        <v>2907</v>
+        <v>2906</v>
       </c>
     </row>
     <row r="274" spans="1:10" x14ac:dyDescent="0.35">
@@ -23420,10 +23420,10 @@
         <v>2423</v>
       </c>
       <c r="E274" s="50" t="s">
-        <v>2912</v>
+        <v>2911</v>
       </c>
       <c r="F274" t="s">
-        <v>2911</v>
+        <v>2910</v>
       </c>
     </row>
     <row r="275" spans="1:10" x14ac:dyDescent="0.35">
@@ -27007,7 +27007,7 @@
     </row>
     <row r="642" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A642" s="16" t="s">
-        <v>2899</v>
+        <v>2898</v>
       </c>
       <c r="E642" t="s">
         <v>2837</v>
@@ -27020,7 +27020,7 @@
     </row>
     <row r="643" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A643" s="16" t="s">
-        <v>2918</v>
+        <v>2917</v>
       </c>
       <c r="E643" t="s">
         <v>1959</v>
@@ -27033,7 +27033,7 @@
     </row>
     <row r="644" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A644" s="16" t="s">
-        <v>2919</v>
+        <v>2918</v>
       </c>
       <c r="E644" t="s">
         <v>1961</v>
@@ -27043,7 +27043,7 @@
     </row>
     <row r="645" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A645" s="16" t="s">
-        <v>2920</v>
+        <v>2919</v>
       </c>
       <c r="E645" t="s">
         <v>1963</v>
@@ -27753,10 +27753,10 @@
         <v>2341</v>
       </c>
       <c r="G34" s="25" t="s">
+        <v>2900</v>
+      </c>
+      <c r="H34" s="25" t="s">
         <v>2901</v>
-      </c>
-      <c r="H34" s="25" t="s">
-        <v>2902</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
@@ -28288,10 +28288,10 @@
         <v>639</v>
       </c>
       <c r="C6" s="32" t="s">
+        <v>2895</v>
+      </c>
+      <c r="D6" t="s">
         <v>2896</v>
-      </c>
-      <c r="D6" t="s">
-        <v>2897</v>
       </c>
       <c r="E6" t="s">
         <v>2157</v>
@@ -34541,10 +34541,10 @@
         <v>639</v>
       </c>
       <c r="C222" s="50" t="s">
+        <v>2904</v>
+      </c>
+      <c r="D222" t="s">
         <v>2905</v>
-      </c>
-      <c r="D222" t="s">
-        <v>2906</v>
       </c>
       <c r="E222" t="s">
         <v>2157</v>
@@ -34570,10 +34570,10 @@
         <v>639</v>
       </c>
       <c r="C223" s="50" t="s">
+        <v>2908</v>
+      </c>
+      <c r="D223" t="s">
         <v>2909</v>
-      </c>
-      <c r="D223" t="s">
-        <v>2910</v>
       </c>
       <c r="E223" t="s">
         <v>2157</v>
@@ -34599,10 +34599,10 @@
         <v>639</v>
       </c>
       <c r="C224" s="50" t="s">
+        <v>2912</v>
+      </c>
+      <c r="D224" t="s">
         <v>2913</v>
-      </c>
-      <c r="D224" t="s">
-        <v>2914</v>
       </c>
       <c r="E224" t="s">
         <v>2157</v>
@@ -34775,7 +34775,7 @@
     </row>
     <row r="231" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A231" s="1" t="s">
-        <v>2898</v>
+        <v>2897</v>
       </c>
       <c r="B231" s="1" t="s">
         <v>2158</v>
@@ -34801,7 +34801,7 @@
     </row>
     <row r="232" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A232" s="1" t="s">
-        <v>2921</v>
+        <v>2920</v>
       </c>
       <c r="B232" s="1" t="s">
         <v>2158</v>
@@ -34827,7 +34827,7 @@
     </row>
     <row r="233" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A233" s="1" t="s">
-        <v>2922</v>
+        <v>2921</v>
       </c>
       <c r="B233" s="1" t="s">
         <v>2158</v>
@@ -34853,7 +34853,7 @@
     </row>
     <row r="234" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A234" s="1" t="s">
-        <v>2923</v>
+        <v>2922</v>
       </c>
       <c r="B234" s="1" t="s">
         <v>2158</v>

</xml_diff>

<commit_message>
update details about UNPD population nature in Value_Type 33
</commit_message>
<xml_diff>
--- a/tmee/data_in/data_dictionary/indicator_dictionary_TM_v5.xlsx
+++ b/tmee/data_in/data_dictionary/indicator_dictionary_TM_v5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/16f1c7c3db740efb/UNICEF/TransMonEE/data-etl/tmee/data_in/data_dictionary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="157" documentId="13_ncr:1_{0D7C4ACD-3B96-48F3-99D4-5E393553EB86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8806B824-3422-47AE-B502-27CA73A00B97}"/>
+  <xr:revisionPtr revIDLastSave="158" documentId="13_ncr:1_{0D7C4ACD-3B96-48F3-99D4-5E393553EB86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{101F90D7-90F4-4ACD-B8AA-B07895A081FC}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Snapshot" sheetId="1" r:id="rId1"/>
@@ -8749,9 +8749,6 @@
     <t>Persons (by sex and age)</t>
   </si>
   <si>
-    <t>Customized for UNPD population. To my best understanding is estimated: have no references about method and frequency of collection</t>
-  </si>
-  <si>
     <t>EDUNF_SAP_L2_GLAST</t>
   </si>
   <si>
@@ -8816,6 +8813,9 @@
   </si>
   <si>
     <t>Total population by age (expressed in thousands)</t>
+  </si>
+  <si>
+    <t>Customized for UNPD population. Not sure if ALL observations are estimated (e.g. OBS_STATUS in Helix are either PR:projections or not specified). Further research: UNPD references about methods and frequency of collection.</t>
   </si>
 </sst>
 </file>
@@ -17072,7 +17072,7 @@
     </row>
     <row r="222" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A222" s="1" t="s">
-        <v>2914</v>
+        <v>2913</v>
       </c>
       <c r="B222" s="16" t="s">
         <v>1443</v>
@@ -17105,7 +17105,7 @@
     </row>
     <row r="223" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A223" s="1" t="s">
-        <v>2915</v>
+        <v>2914</v>
       </c>
       <c r="B223" s="16" t="s">
         <v>1818</v>
@@ -17138,7 +17138,7 @@
     </row>
     <row r="224" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A224" s="1" t="s">
-        <v>2916</v>
+        <v>2915</v>
       </c>
       <c r="B224" s="16" t="s">
         <v>1820</v>
@@ -17706,7 +17706,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M645"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E23" sqref="E23"/>
     </sheetView>
@@ -18284,7 +18284,7 @@
         <v>2893</v>
       </c>
       <c r="E23" s="33" t="s">
-        <v>2923</v>
+        <v>2922</v>
       </c>
       <c r="F23" s="56" t="s">
         <v>2894</v>
@@ -23380,10 +23380,10 @@
         <v>2843</v>
       </c>
       <c r="E272" s="50" t="s">
-        <v>2903</v>
+        <v>2902</v>
       </c>
       <c r="F272" t="s">
-        <v>2902</v>
+        <v>2901</v>
       </c>
     </row>
     <row r="273" spans="1:10" x14ac:dyDescent="0.35">
@@ -23400,10 +23400,10 @@
         <v>2423</v>
       </c>
       <c r="E273" s="50" t="s">
-        <v>2907</v>
+        <v>2906</v>
       </c>
       <c r="F273" t="s">
-        <v>2906</v>
+        <v>2905</v>
       </c>
     </row>
     <row r="274" spans="1:10" x14ac:dyDescent="0.35">
@@ -23420,10 +23420,10 @@
         <v>2423</v>
       </c>
       <c r="E274" s="50" t="s">
-        <v>2911</v>
+        <v>2910</v>
       </c>
       <c r="F274" t="s">
-        <v>2910</v>
+        <v>2909</v>
       </c>
     </row>
     <row r="275" spans="1:10" x14ac:dyDescent="0.35">
@@ -27020,7 +27020,7 @@
     </row>
     <row r="643" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A643" s="16" t="s">
-        <v>2917</v>
+        <v>2916</v>
       </c>
       <c r="E643" t="s">
         <v>1959</v>
@@ -27033,7 +27033,7 @@
     </row>
     <row r="644" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A644" s="16" t="s">
-        <v>2918</v>
+        <v>2917</v>
       </c>
       <c r="E644" t="s">
         <v>1961</v>
@@ -27043,7 +27043,7 @@
     </row>
     <row r="645" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A645" s="16" t="s">
-        <v>2919</v>
+        <v>2918</v>
       </c>
       <c r="E645" t="s">
         <v>1963</v>
@@ -27067,8 +27067,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K107"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -27756,7 +27756,7 @@
         <v>2900</v>
       </c>
       <c r="H34" s="25" t="s">
-        <v>2901</v>
+        <v>2923</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
@@ -34541,10 +34541,10 @@
         <v>639</v>
       </c>
       <c r="C222" s="50" t="s">
+        <v>2903</v>
+      </c>
+      <c r="D222" t="s">
         <v>2904</v>
-      </c>
-      <c r="D222" t="s">
-        <v>2905</v>
       </c>
       <c r="E222" t="s">
         <v>2157</v>
@@ -34570,10 +34570,10 @@
         <v>639</v>
       </c>
       <c r="C223" s="50" t="s">
+        <v>2907</v>
+      </c>
+      <c r="D223" t="s">
         <v>2908</v>
-      </c>
-      <c r="D223" t="s">
-        <v>2909</v>
       </c>
       <c r="E223" t="s">
         <v>2157</v>
@@ -34599,10 +34599,10 @@
         <v>639</v>
       </c>
       <c r="C224" s="50" t="s">
+        <v>2911</v>
+      </c>
+      <c r="D224" t="s">
         <v>2912</v>
-      </c>
-      <c r="D224" t="s">
-        <v>2913</v>
       </c>
       <c r="E224" t="s">
         <v>2157</v>
@@ -34801,7 +34801,7 @@
     </row>
     <row r="232" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A232" s="1" t="s">
-        <v>2920</v>
+        <v>2919</v>
       </c>
       <c r="B232" s="1" t="s">
         <v>2158</v>
@@ -34827,7 +34827,7 @@
     </row>
     <row r="233" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A233" s="1" t="s">
-        <v>2921</v>
+        <v>2920</v>
       </c>
       <c r="B233" s="1" t="s">
         <v>2158</v>
@@ -34853,7 +34853,7 @@
     </row>
     <row r="234" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A234" s="1" t="s">
-        <v>2922</v>
+        <v>2921</v>
       </c>
       <c r="B234" s="1" t="s">
         <v>2158</v>

</xml_diff>